<commit_message>
Update data to 27 February 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="297">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -905,6 +905,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240226082300/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.02.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240227062937/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1005,15 +1011,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M142"/>
+  <dimension ref="A1:M143"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1695" topLeftCell="A130" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="690" topLeftCell="A130" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M142" activeCellId="0" sqref="M142"/>
+      <selection pane="bottomLeft" activeCell="M143" activeCellId="0" sqref="M143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6137,6 +6143,47 @@
       </c>
       <c r="M142" s="0" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="C143" s="0" t="n">
+        <v>29782</v>
+      </c>
+      <c r="D143" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E143" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F143" s="0" t="n">
+        <v>70043</v>
+      </c>
+      <c r="G143" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H143" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I143" s="0" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J143" s="0" t="n">
+        <v>407</v>
+      </c>
+      <c r="K143" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="L143" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M143" s="0" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to 29 February
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="301">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -910,7 +910,19 @@
     <t xml:space="preserve">27.02.2024</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20240227062937/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+    <t xml:space="preserve">https://web.archive.org/web/20240227162215/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.02.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240228183950/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.02.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240229162901/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1011,15 +1023,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M143"/>
+  <dimension ref="A1:M145"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="690" topLeftCell="A130" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="705" topLeftCell="A122" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M143" activeCellId="0" sqref="M143"/>
+      <selection pane="bottomLeft" activeCell="I148" activeCellId="0" sqref="I148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6153,7 +6165,7 @@
         <v>295</v>
       </c>
       <c r="C143" s="0" t="n">
-        <v>29782</v>
+        <v>29878</v>
       </c>
       <c r="D143" s="0" t="n">
         <v>12300</v>
@@ -6162,7 +6174,7 @@
         <v>8400</v>
       </c>
       <c r="F143" s="0" t="n">
-        <v>70043</v>
+        <v>70215</v>
       </c>
       <c r="G143" s="0" t="n">
         <v>8663</v>
@@ -6184,6 +6196,88 @@
       </c>
       <c r="M143" s="0" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="C144" s="0" t="n">
+        <v>29954</v>
+      </c>
+      <c r="D144" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E144" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F144" s="0" t="n">
+        <v>70325</v>
+      </c>
+      <c r="G144" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H144" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I144" s="0" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J144" s="0" t="n">
+        <v>411</v>
+      </c>
+      <c r="K144" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="L144" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M144" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <v>30035</v>
+      </c>
+      <c r="D145" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E145" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F145" s="0" t="n">
+        <v>70457</v>
+      </c>
+      <c r="G145" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H145" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I145" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J145" s="0" t="n">
+        <v>414</v>
+      </c>
+      <c r="K145" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="L145" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M145" s="0" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to account for 1 March 2024 data
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="303">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -923,6 +923,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240229162901/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240301162100/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1023,15 +1029,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M145"/>
+  <dimension ref="A1:M146"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="705" topLeftCell="A122" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1770" topLeftCell="A122" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I148" activeCellId="0" sqref="I148"/>
+      <selection pane="bottomLeft" activeCell="M146" activeCellId="0" sqref="M146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6278,6 +6284,47 @@
       </c>
       <c r="M145" s="0" t="s">
         <v>300</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C146" s="0" t="n">
+        <v>30228</v>
+      </c>
+      <c r="D146" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E146" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F146" s="0" t="n">
+        <v>71377</v>
+      </c>
+      <c r="G146" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H146" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I146" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J146" s="0" t="n">
+        <v>417</v>
+      </c>
+      <c r="K146" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="L146" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M146" s="0" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for data on 4 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="309">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -929,6 +929,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240301162100/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240302133451/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240303020113/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated from the tracker</t>
   </si>
 </sst>
 </file>
@@ -1029,15 +1047,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M146"/>
+  <dimension ref="A1:M149"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1770" topLeftCell="A122" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="675" topLeftCell="A122" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M146" activeCellId="0" sqref="M146"/>
+      <selection pane="bottomLeft" activeCell="A150" activeCellId="0" sqref="A150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6325,6 +6343,129 @@
       </c>
       <c r="M146" s="0" t="s">
         <v>302</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C147" s="0" t="n">
+        <v>30228</v>
+      </c>
+      <c r="D147" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E147" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F147" s="0" t="n">
+        <v>71377</v>
+      </c>
+      <c r="G147" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H147" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I147" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J147" s="0" t="n">
+        <v>417</v>
+      </c>
+      <c r="K147" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="L147" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M147" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C148" s="0" t="n">
+        <v>30228</v>
+      </c>
+      <c r="D148" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E148" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F148" s="0" t="n">
+        <v>71377</v>
+      </c>
+      <c r="G148" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H148" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I148" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J148" s="0" t="n">
+        <v>417</v>
+      </c>
+      <c r="K148" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="L148" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M148" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="C149" s="0" t="n">
+        <v>30534</v>
+      </c>
+      <c r="D149" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E149" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <v>71920</v>
+      </c>
+      <c r="G149" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H149" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I149" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J149" s="0" t="n">
+        <v>420</v>
+      </c>
+      <c r="K149" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="L149" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M149" s="0" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Provided wayback machine reference for 4 Macrh 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -946,7 +946,7 @@
     <t xml:space="preserve">04.04.2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Updated from the tracker</t>
+    <t xml:space="preserve">https://web.archive.org/web/20240304220143/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1050,12 +1050,12 @@
   <dimension ref="A1:M149"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="675" topLeftCell="A122" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="585" topLeftCell="A122" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A150" activeCellId="0" sqref="A150"/>
+      <selection pane="bottomLeft" activeCell="M149" activeCellId="0" sqref="M149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Update data for 05 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="311">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -947,6 +947,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240304220143/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240305152521/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1047,15 +1053,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M149"/>
+  <dimension ref="A1:M150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="585" topLeftCell="A122" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="705" topLeftCell="A122" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M149" activeCellId="0" sqref="M149"/>
+      <selection pane="bottomLeft" activeCell="A151" activeCellId="0" sqref="A151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6466,6 +6472,47 @@
       </c>
       <c r="M149" s="0" t="s">
         <v>308</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C150" s="0" t="n">
+        <v>30631</v>
+      </c>
+      <c r="D150" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E150" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F150" s="0" t="n">
+        <v>72043</v>
+      </c>
+      <c r="G150" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H150" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I150" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J150" s="0" t="n">
+        <v>421</v>
+      </c>
+      <c r="K150" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="L150" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M150" s="0" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 06 March 2024 data
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="313">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -953,6 +953,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240305152521/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240306153510/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1053,15 +1059,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M150"/>
+  <dimension ref="A1:M151"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="705" topLeftCell="A122" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="990" topLeftCell="A142" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A151" activeCellId="0" sqref="A151"/>
+      <selection pane="bottomLeft" activeCell="M151" activeCellId="0" sqref="M151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6513,6 +6519,47 @@
       </c>
       <c r="M150" s="0" t="s">
         <v>310</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="C151" s="0" t="n">
+        <v>30717</v>
+      </c>
+      <c r="D151" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E151" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F151" s="0" t="n">
+        <v>72156</v>
+      </c>
+      <c r="G151" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H151" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I151" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J151" s="0" t="n">
+        <v>423</v>
+      </c>
+      <c r="K151" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="L151" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M151" s="0" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 10 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="321">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -959,6 +959,30 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240306153510/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240307133101/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240308174707/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240309192855/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240310134417/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1059,15 +1083,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M151"/>
+  <dimension ref="A1:M155"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="990" topLeftCell="A142" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="765" topLeftCell="A129" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M151" activeCellId="0" sqref="M151"/>
+      <selection pane="bottomLeft" activeCell="M155" activeCellId="0" sqref="M155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6560,6 +6584,170 @@
       </c>
       <c r="M151" s="0" t="s">
         <v>312</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>30800</v>
+      </c>
+      <c r="D152" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E152" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F152" s="0" t="n">
+        <v>72298</v>
+      </c>
+      <c r="G152" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H152" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I152" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J152" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="K152" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="L152" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M152" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C153" s="0" t="n">
+        <v>30878</v>
+      </c>
+      <c r="D153" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E153" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F153" s="0" t="n">
+        <v>72402</v>
+      </c>
+      <c r="G153" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H153" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I153" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J153" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="K153" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="L153" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M153" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C154" s="0" t="n">
+        <v>30878</v>
+      </c>
+      <c r="D154" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E154" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F154" s="0" t="n">
+        <v>72402</v>
+      </c>
+      <c r="G154" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H154" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I154" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J154" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="K154" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="L154" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="M154" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="C155" s="0" t="n">
+        <v>31045</v>
+      </c>
+      <c r="D155" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E155" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F155" s="0" t="n">
+        <v>72654</v>
+      </c>
+      <c r="G155" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H155" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I155" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J155" s="0" t="n">
+        <v>425</v>
+      </c>
+      <c r="K155" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="L155" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M155" s="0" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 13 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="327">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -983,6 +983,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240310134417/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240311174900/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240312034827/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240313155810/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1083,15 +1101,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M155"/>
+  <dimension ref="A1:M158"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="765" topLeftCell="A129" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="735" topLeftCell="A135" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M155" activeCellId="0" sqref="M155"/>
+      <selection pane="bottomLeft" activeCell="K160" activeCellId="0" sqref="K160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6748,6 +6766,129 @@
       </c>
       <c r="M155" s="0" t="s">
         <v>320</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="C156" s="0" t="n">
+        <v>31045</v>
+      </c>
+      <c r="D156" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E156" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F156" s="0" t="n">
+        <v>72654</v>
+      </c>
+      <c r="G156" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H156" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I156" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J156" s="0" t="n">
+        <v>425</v>
+      </c>
+      <c r="K156" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="L156" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M156" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="C157" s="0" t="n">
+        <v>31045</v>
+      </c>
+      <c r="D157" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E157" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F157" s="0" t="n">
+        <v>72654</v>
+      </c>
+      <c r="G157" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H157" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I157" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J157" s="0" t="n">
+        <v>425</v>
+      </c>
+      <c r="K157" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="L157" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M157" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C158" s="0" t="n">
+        <v>31272</v>
+      </c>
+      <c r="D158" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E158" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F158" s="0" t="n">
+        <v>73024</v>
+      </c>
+      <c r="G158" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H158" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I158" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J158" s="0" t="n">
+        <v>432</v>
+      </c>
+      <c r="K158" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="L158" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M158" s="0" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 15 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="331">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1001,6 +1001,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240313155810/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240314205339/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240315162911/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1101,15 +1113,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M158"/>
+  <dimension ref="A1:M160"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="735" topLeftCell="A135" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K160" activeCellId="0" sqref="K160"/>
+      <selection pane="bottomLeft" activeCell="M159" activeCellId="0" sqref="M159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6889,6 +6901,88 @@
       </c>
       <c r="M158" s="0" t="s">
         <v>326</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="C159" s="0" t="n">
+        <v>31341</v>
+      </c>
+      <c r="D159" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E159" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F159" s="0" t="n">
+        <v>73134</v>
+      </c>
+      <c r="G159" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H159" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I159" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J159" s="0" t="n">
+        <v>433</v>
+      </c>
+      <c r="K159" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L159" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M159" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="C160" s="0" t="n">
+        <v>31490</v>
+      </c>
+      <c r="D160" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E160" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F160" s="0" t="n">
+        <v>73439</v>
+      </c>
+      <c r="G160" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H160" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I160" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J160" s="0" t="n">
+        <v>433</v>
+      </c>
+      <c r="K160" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L160" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M160" s="0" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Date and images updated using data up until 17 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="335">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1013,6 +1013,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240315162911/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240316233943/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240317121641/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1113,15 +1125,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M160"/>
+  <dimension ref="A1:M162"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="735" topLeftCell="A135" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="765" topLeftCell="A144" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M159" activeCellId="0" sqref="M159"/>
+      <selection pane="bottomLeft" activeCell="M162" activeCellId="0" sqref="M162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -6983,6 +6995,88 @@
       </c>
       <c r="M160" s="0" t="s">
         <v>330</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="C161" s="0" t="n">
+        <v>31490</v>
+      </c>
+      <c r="D161" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E161" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F161" s="0" t="n">
+        <v>73439</v>
+      </c>
+      <c r="G161" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H161" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I161" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J161" s="0" t="n">
+        <v>433</v>
+      </c>
+      <c r="K161" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L161" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M161" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="C162" s="0" t="n">
+        <v>31490</v>
+      </c>
+      <c r="D162" s="0" t="n">
+        <v>12300</v>
+      </c>
+      <c r="E162" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F162" s="0" t="n">
+        <v>73439</v>
+      </c>
+      <c r="G162" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H162" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I162" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J162" s="0" t="n">
+        <v>433</v>
+      </c>
+      <c r="K162" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L162" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M162" s="0" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 18 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="337">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1025,6 +1025,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240317121641/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240318235631/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1040,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1055,6 +1061,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1099,12 +1112,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1125,15 +1142,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M162"/>
+  <dimension ref="A1:M163"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="765" topLeftCell="A144" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="2025" topLeftCell="A144" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M162" activeCellId="0" sqref="M162"/>
+      <selection pane="bottomLeft" activeCell="M163" activeCellId="0" sqref="M163"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7077,6 +7094,47 @@
       </c>
       <c r="M162" s="0" t="s">
         <v>334</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="C163" s="0" t="n">
+        <v>31726</v>
+      </c>
+      <c r="D163" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E163" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F163" s="0" t="n">
+        <v>73729</v>
+      </c>
+      <c r="G163" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H163" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I163" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J163" s="0" t="n">
+        <v>435</v>
+      </c>
+      <c r="K163" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L163" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M163" s="2" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 19 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="339">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1031,6 +1031,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240318235631/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240319204452/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1142,15 +1148,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M163"/>
+  <dimension ref="A1:M164"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2025" topLeftCell="A144" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="720" topLeftCell="A144" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M163" activeCellId="0" sqref="M163"/>
+      <selection pane="bottomLeft" activeCell="M164" activeCellId="0" sqref="M164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7135,6 +7141,47 @@
       </c>
       <c r="M163" s="2" t="s">
         <v>336</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="C164" s="0" t="n">
+        <v>31726</v>
+      </c>
+      <c r="D164" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E164" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F164" s="0" t="n">
+        <v>73729</v>
+      </c>
+      <c r="G164" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H164" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I164" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J164" s="0" t="n">
+        <v>435</v>
+      </c>
+      <c r="K164" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L164" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M164" s="0" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 20 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="341">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1037,6 +1037,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240319204452/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240320153709/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1148,15 +1154,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M164"/>
+  <dimension ref="A1:M165"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="720" topLeftCell="A144" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="660" topLeftCell="A144" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M164" activeCellId="0" sqref="M164"/>
+      <selection pane="bottomLeft" activeCell="M165" activeCellId="0" sqref="M165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7182,6 +7188,47 @@
       </c>
       <c r="M164" s="0" t="s">
         <v>338</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="C165" s="0" t="n">
+        <v>31923</v>
+      </c>
+      <c r="D165" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E165" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F165" s="0" t="n">
+        <v>74096</v>
+      </c>
+      <c r="G165" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H165" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I165" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J165" s="0" t="n">
+        <v>437</v>
+      </c>
+      <c r="K165" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L165" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M165" s="0" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upated the data on 21 March 2024, and corrected an error on the date for the data for 04 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="343">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -943,7 +943,7 @@
     <t xml:space="preserve">https://web.archive.org/web/20240303020113/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
   <si>
-    <t xml:space="preserve">04.04.2024</t>
+    <t xml:space="preserve">04.03.2024</t>
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240304220143/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
@@ -1043,6 +1043,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240320153709/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240321141457/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1154,15 +1160,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M165"/>
+  <dimension ref="A1:M166"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="660" topLeftCell="A144" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="720" topLeftCell="A150" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M165" activeCellId="0" sqref="M165"/>
+      <selection pane="bottomLeft" activeCell="M166" activeCellId="0" sqref="M166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7229,6 +7235,47 @@
       </c>
       <c r="M165" s="0" t="s">
         <v>340</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="C166" s="0" t="n">
+        <v>31988</v>
+      </c>
+      <c r="D166" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E166" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F166" s="0" t="n">
+        <v>74188</v>
+      </c>
+      <c r="G166" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H166" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I166" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J166" s="0" t="n">
+        <v>442</v>
+      </c>
+      <c r="K166" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L166" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M166" s="0" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 22 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="345">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1049,6 +1049,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240321141457/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240322181740/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1160,15 +1166,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M166"/>
+  <dimension ref="A1:M167"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="720" topLeftCell="A150" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="2025" topLeftCell="A150" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M166" activeCellId="0" sqref="M166"/>
+      <selection pane="bottomLeft" activeCell="L171" activeCellId="0" sqref="L171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7276,6 +7282,47 @@
       </c>
       <c r="M166" s="0" t="s">
         <v>342</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>32070</v>
+      </c>
+      <c r="D167" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="E167" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F167" s="0" t="n">
+        <v>74298</v>
+      </c>
+      <c r="G167" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H167" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I167" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J167" s="0" t="n">
+        <v>442</v>
+      </c>
+      <c r="K167" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L167" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M167" s="0" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected an error in the updated child deaths on 22 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -1169,12 +1169,12 @@
   <dimension ref="A1:M167"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2025" topLeftCell="A150" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="675" topLeftCell="A150" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L171" activeCellId="0" sqref="L171"/>
+      <selection pane="bottomLeft" activeCell="A173" activeCellId="0" sqref="A173"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7295,7 +7295,7 @@
         <v>32070</v>
       </c>
       <c r="D167" s="0" t="n">
-        <v>1300</v>
+        <v>13000</v>
       </c>
       <c r="E167" s="0" t="n">
         <v>8400</v>

</xml_diff>

<commit_message>
Update 24 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="349">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1055,6 +1055,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240322181740/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240323053658/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240324191339/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1148,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1147,6 +1159,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1166,15 +1182,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M167"/>
+  <dimension ref="A1:M169"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="675" topLeftCell="A150" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="945" topLeftCell="A150" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A173" activeCellId="0" sqref="A173"/>
+      <selection pane="bottomLeft" activeCell="M169" activeCellId="0" sqref="M169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7323,6 +7339,88 @@
       </c>
       <c r="M167" s="0" t="s">
         <v>344</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="C168" s="0" t="n">
+        <v>32070</v>
+      </c>
+      <c r="D168" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E168" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F168" s="0" t="n">
+        <v>74298</v>
+      </c>
+      <c r="G168" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H168" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I168" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J168" s="0" t="n">
+        <v>442</v>
+      </c>
+      <c r="K168" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L168" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M168" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <v>32226</v>
+      </c>
+      <c r="D169" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E169" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F169" s="3" t="n">
+        <v>74518</v>
+      </c>
+      <c r="G169" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H169" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I169" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J169" s="0" t="n">
+        <v>442</v>
+      </c>
+      <c r="K169" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L169" s="0" t="n">
+        <v>4700</v>
+      </c>
+      <c r="M169" s="0" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 26 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="353">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1067,6 +1067,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240324191339/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240325135227/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240326214610/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1182,15 +1194,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M169"/>
+  <dimension ref="A1:M171"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="945" topLeftCell="A150" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="720" topLeftCell="A156" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M169" activeCellId="0" sqref="M169"/>
+      <selection pane="bottomLeft" activeCell="M171" activeCellId="0" sqref="M171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7421,6 +7433,88 @@
       </c>
       <c r="M169" s="0" t="s">
         <v>348</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="C170" s="3" t="n">
+        <v>32333</v>
+      </c>
+      <c r="D170" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E170" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F170" s="3" t="n">
+        <v>74694</v>
+      </c>
+      <c r="G170" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H170" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I170" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J170" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="K170" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L170" s="0" t="n">
+        <v>4700</v>
+      </c>
+      <c r="M170" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="C171" s="3" t="n">
+        <v>32333</v>
+      </c>
+      <c r="D171" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E171" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F171" s="3" t="n">
+        <v>74694</v>
+      </c>
+      <c r="G171" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H171" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I171" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J171" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="K171" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L171" s="0" t="n">
+        <v>4700</v>
+      </c>
+      <c r="M171" s="0" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 27 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="355">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1079,6 +1079,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240326214610/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240327142318/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1194,15 +1200,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M171"/>
+  <dimension ref="A1:M172"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="720" topLeftCell="A156" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1005" topLeftCell="A156" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M171" activeCellId="0" sqref="M171"/>
+      <selection pane="bottomLeft" activeCell="L175" activeCellId="0" sqref="L175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7515,6 +7521,47 @@
       </c>
       <c r="M171" s="0" t="s">
         <v>352</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="C172" s="0" t="n">
+        <v>32490</v>
+      </c>
+      <c r="D172" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E172" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F172" s="0" t="n">
+        <v>74889</v>
+      </c>
+      <c r="G172" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H172" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I172" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J172" s="0" t="n">
+        <v>453</v>
+      </c>
+      <c r="K172" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L172" s="0" t="n">
+        <v>4700</v>
+      </c>
+      <c r="M172" s="0" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 28 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="357">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1085,6 +1085,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240327142318/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240328175507/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1200,15 +1206,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M172"/>
+  <dimension ref="A1:M173"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1005" topLeftCell="A156" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="720" topLeftCell="A156" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L175" activeCellId="0" sqref="L175"/>
+      <selection pane="bottomLeft" activeCell="M177" activeCellId="0" sqref="M177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7562,6 +7568,47 @@
       </c>
       <c r="M172" s="0" t="s">
         <v>354</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="C173" s="3" t="n">
+        <v>32552</v>
+      </c>
+      <c r="D173" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E173" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F173" s="0" t="n">
+        <v>74980</v>
+      </c>
+      <c r="G173" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H173" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I173" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J173" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="K173" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L173" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M173" s="0" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to 31 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="363">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1091,6 +1091,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240328175507/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240329155650/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240330182428/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.03.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240331170708/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1206,15 +1224,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M173"/>
+  <dimension ref="A1:M176"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="720" topLeftCell="A156" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1290" topLeftCell="A156" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M177" activeCellId="0" sqref="M177"/>
+      <selection pane="bottomLeft" activeCell="A177" activeCellId="0" sqref="A177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7609,6 +7627,129 @@
       </c>
       <c r="M173" s="0" t="s">
         <v>356</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <v>32623</v>
+      </c>
+      <c r="D174" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E174" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F174" s="0" t="n">
+        <v>75092</v>
+      </c>
+      <c r="G174" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H174" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I174" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J174" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="K174" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L174" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M174" s="0" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="C175" s="0" t="n">
+        <v>32623</v>
+      </c>
+      <c r="D175" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E175" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F175" s="0" t="n">
+        <v>75092</v>
+      </c>
+      <c r="G175" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H175" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I175" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J175" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="K175" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L175" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M175" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="C176" s="0" t="n">
+        <v>32782</v>
+      </c>
+      <c r="D176" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E176" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F176" s="0" t="n">
+        <v>75298</v>
+      </c>
+      <c r="G176" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H176" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I176" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J176" s="0" t="n">
+        <v>455</v>
+      </c>
+      <c r="K176" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="L176" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M176" s="0" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 02 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="367">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1109,6 +1109,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240331170708/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240402082823/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240402173216/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1224,15 +1236,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M176"/>
+  <dimension ref="A1:M178"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1290" topLeftCell="A156" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="780" topLeftCell="A164" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A177" activeCellId="0" sqref="A177"/>
+      <selection pane="bottomLeft" activeCell="M178" activeCellId="0" sqref="M178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7750,6 +7762,88 @@
       </c>
       <c r="M176" s="0" t="s">
         <v>362</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>32845</v>
+      </c>
+      <c r="D177" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E177" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F177" s="0" t="n">
+        <v>75392</v>
+      </c>
+      <c r="G177" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H177" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I177" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J177" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="K177" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L177" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M177" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="C178" s="0" t="n">
+        <v>32845</v>
+      </c>
+      <c r="D178" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E178" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F178" s="0" t="n">
+        <v>75392</v>
+      </c>
+      <c r="G178" s="0" t="n">
+        <v>8663</v>
+      </c>
+      <c r="H178" s="0" t="n">
+        <v>6327</v>
+      </c>
+      <c r="I178" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J178" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="K178" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L178" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M178" s="0" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 03 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="369">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1121,6 +1121,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240402173216/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240403192225/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1236,15 +1242,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M178"/>
+  <dimension ref="A1:M179"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="780" topLeftCell="A164" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1410" topLeftCell="A164" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M178" activeCellId="0" sqref="M178"/>
+      <selection pane="bottomLeft" activeCell="M179" activeCellId="0" sqref="M179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7844,6 +7850,41 @@
       </c>
       <c r="M178" s="0" t="s">
         <v>366</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="C179" s="0" t="n">
+        <v>32975</v>
+      </c>
+      <c r="D179" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E179" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F179" s="0" t="n">
+        <v>75577</v>
+      </c>
+      <c r="I179" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J179" s="0" t="n">
+        <v>457</v>
+      </c>
+      <c r="K179" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L179" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M179" s="0" t="s">
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 05 March 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="373">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1127,6 +1127,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240403192225/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240404230708/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240405151423/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1242,15 +1254,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M179"/>
+  <dimension ref="A1:M181"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1410" topLeftCell="A164" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1350" topLeftCell="A164" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M179" activeCellId="0" sqref="M179"/>
+      <selection pane="bottomLeft" activeCell="K185" activeCellId="0" sqref="K185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7885,6 +7897,76 @@
       </c>
       <c r="M179" s="0" t="s">
         <v>368</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C180" s="0" t="n">
+        <v>33037</v>
+      </c>
+      <c r="D180" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E180" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F180" s="0" t="n">
+        <v>75668</v>
+      </c>
+      <c r="I180" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J180" s="0" t="n">
+        <v>457</v>
+      </c>
+      <c r="K180" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L180" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M180" s="0" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C181" s="0" t="n">
+        <v>33037</v>
+      </c>
+      <c r="D181" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E181" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F181" s="0" t="n">
+        <v>75668</v>
+      </c>
+      <c r="I181" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J181" s="0" t="n">
+        <v>457</v>
+      </c>
+      <c r="K181" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L181" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M181" s="0" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 6 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="375">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1139,6 +1139,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240405151423/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240406170548/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1254,15 +1260,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M181"/>
+  <dimension ref="A1:M182"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1350" topLeftCell="A164" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="2430" topLeftCell="A164" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K185" activeCellId="0" sqref="K185"/>
+      <selection pane="bottomLeft" activeCell="M182" activeCellId="0" sqref="M182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7967,6 +7973,41 @@
       </c>
       <c r="M181" s="0" t="s">
         <v>372</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C182" s="0" t="n">
+        <v>33137</v>
+      </c>
+      <c r="D182" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E182" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F182" s="0" t="n">
+        <v>75815</v>
+      </c>
+      <c r="I182" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J182" s="0" t="n">
+        <v>459</v>
+      </c>
+      <c r="K182" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L182" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M182" s="0" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 7 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="377">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1145,6 +1145,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240406170548/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240407140639/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1260,15 +1266,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M182"/>
+  <dimension ref="A1:M183"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2430" topLeftCell="A164" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="930" topLeftCell="A161" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M182" activeCellId="0" sqref="M182"/>
+      <selection pane="bottomLeft" activeCell="M183" activeCellId="0" sqref="M183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8008,6 +8014,41 @@
       </c>
       <c r="M182" s="0" t="s">
         <v>374</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C183" s="0" t="n">
+        <v>33175</v>
+      </c>
+      <c r="D183" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E183" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F183" s="0" t="n">
+        <v>75886</v>
+      </c>
+      <c r="I183" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J183" s="0" t="n">
+        <v>459</v>
+      </c>
+      <c r="K183" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L183" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M183" s="0" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with data from 9 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="381">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1151,6 +1151,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240407140639/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240408232546/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240410001454/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1266,15 +1278,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M183"/>
+  <dimension ref="A1:M185"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="930" topLeftCell="A161" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1680" topLeftCell="A38" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M183" activeCellId="0" sqref="M183"/>
+      <selection pane="bottomLeft" activeCell="I184" activeCellId="0" sqref="I184:J184"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8049,6 +8061,76 @@
       </c>
       <c r="M183" s="0" t="s">
         <v>376</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C184" s="0" t="n">
+        <v>33175</v>
+      </c>
+      <c r="D184" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E184" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F184" s="0" t="n">
+        <v>75886</v>
+      </c>
+      <c r="I184" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J184" s="0" t="n">
+        <v>459</v>
+      </c>
+      <c r="K184" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L184" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M184" s="0" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="C185" s="0" t="n">
+        <v>33027</v>
+      </c>
+      <c r="D185" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E185" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F185" s="0" t="n">
+        <v>75933</v>
+      </c>
+      <c r="I185" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J185" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="K185" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L185" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M185" s="0" t="s">
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 11 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="385">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1163,6 +1163,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240410001454/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240410224411/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240411182552/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1278,15 +1290,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M185"/>
+  <dimension ref="A1:M187"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1680" topLeftCell="A38" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1350" topLeftCell="A173" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I184" activeCellId="0" sqref="I184:J184"/>
+      <selection pane="bottomLeft" activeCell="D187" activeCellId="0" sqref="D187"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8106,7 +8118,7 @@
         <v>379</v>
       </c>
       <c r="C185" s="0" t="n">
-        <v>33027</v>
+        <v>33207</v>
       </c>
       <c r="D185" s="0" t="n">
         <v>13000</v>
@@ -8131,6 +8143,76 @@
       </c>
       <c r="M185" s="0" t="s">
         <v>380</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="B186" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="C186" s="0" t="n">
+        <v>33482</v>
+      </c>
+      <c r="D186" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E186" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F186" s="0" t="n">
+        <v>76049</v>
+      </c>
+      <c r="I186" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J186" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="K186" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L186" s="0" t="n">
+        <v>4650</v>
+      </c>
+      <c r="M186" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="C187" s="0" t="n">
+        <v>33545</v>
+      </c>
+      <c r="D187" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E187" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F187" s="0" t="n">
+        <v>76094</v>
+      </c>
+      <c r="I187" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J187" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="K187" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L187" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M187" s="0" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 14 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="391">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1175,6 +1175,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240411182552/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240412232348/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240413105351/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240414152645/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1290,15 +1308,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M187"/>
+  <dimension ref="A1:M190"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1350" topLeftCell="A173" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D187" activeCellId="0" sqref="D187"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1215" topLeftCell="A186" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="M190" activeCellId="0" sqref="M190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8213,6 +8231,111 @@
       </c>
       <c r="M187" s="0" t="s">
         <v>384</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="C188" s="0" t="n">
+        <v>33634</v>
+      </c>
+      <c r="D188" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E188" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F188" s="0" t="n">
+        <v>76214</v>
+      </c>
+      <c r="I188" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J188" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="K188" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L188" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M188" s="0" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B189" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="C189" s="0" t="n">
+        <v>33634</v>
+      </c>
+      <c r="D189" s="0" t="n">
+        <v>13000</v>
+      </c>
+      <c r="E189" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F189" s="0" t="n">
+        <v>76214</v>
+      </c>
+      <c r="I189" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J189" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="K189" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="L189" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M189" s="0" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B190" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="C190" s="0" t="n">
+        <v>33729</v>
+      </c>
+      <c r="D190" s="0" t="n">
+        <v>13800</v>
+      </c>
+      <c r="E190" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F190" s="0" t="n">
+        <v>76371</v>
+      </c>
+      <c r="I190" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J190" s="0" t="n">
+        <v>465</v>
+      </c>
+      <c r="K190" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="L190" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M190" s="0" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 17 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="397">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1193,6 +1193,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240414152645/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240415190656/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240416235054/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240417103234/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1308,15 +1326,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M190"/>
+  <dimension ref="A1:M193"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1215" topLeftCell="A186" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="M190" activeCellId="0" sqref="M190"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="660" topLeftCell="A186" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="K198" activeCellId="0" sqref="K198"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8336,6 +8354,111 @@
       </c>
       <c r="M190" s="0" t="s">
         <v>390</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B191" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="C191" s="3" t="n">
+        <v>33797</v>
+      </c>
+      <c r="D191" s="0" t="n">
+        <v>13800</v>
+      </c>
+      <c r="E191" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F191" s="3" t="n">
+        <v>76465</v>
+      </c>
+      <c r="I191" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J191" s="0" t="n">
+        <v>465</v>
+      </c>
+      <c r="K191" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="L191" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M191" s="0" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="B192" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="C192" s="3" t="n">
+        <v>33797</v>
+      </c>
+      <c r="D192" s="0" t="n">
+        <v>13800</v>
+      </c>
+      <c r="E192" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F192" s="3" t="n">
+        <v>76465</v>
+      </c>
+      <c r="I192" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J192" s="0" t="n">
+        <v>465</v>
+      </c>
+      <c r="K192" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="L192" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M192" s="0" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B193" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="C193" s="3" t="n">
+        <v>33899</v>
+      </c>
+      <c r="D193" s="0" t="n">
+        <v>13800</v>
+      </c>
+      <c r="E193" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F193" s="3" t="n">
+        <v>76664</v>
+      </c>
+      <c r="I193" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J193" s="0" t="n">
+        <v>468</v>
+      </c>
+      <c r="K193" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="L193" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M193" s="0" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 21 April 2024. The WayBackMachine failed to save the Aljazeera tracking site correctly. It recorded the latest casualty figures as of April 21 at 2:30pm in Gaza (11:30 GMT) as saved but the latest page points to something saved 2 hours earlier that is from 19 April: https://web.archive.org/web/20240421121235/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="404">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1211,6 +1211,27 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240417103234/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240418215003/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240419203633/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240420210539/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.04.2024</t>
   </si>
 </sst>
 </file>
@@ -1326,15 +1347,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M193"/>
+  <dimension ref="A1:M197"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="660" topLeftCell="A186" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K198" activeCellId="0" sqref="K198"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2130" topLeftCell="A186" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="M204" activeCellId="0" sqref="M204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8459,6 +8480,143 @@
       </c>
       <c r="M193" s="0" t="s">
         <v>396</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B194" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="C194" s="3" t="n">
+        <v>33899</v>
+      </c>
+      <c r="D194" s="0" t="n">
+        <v>13800</v>
+      </c>
+      <c r="E194" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F194" s="3" t="n">
+        <v>76664</v>
+      </c>
+      <c r="I194" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J194" s="0" t="n">
+        <v>468</v>
+      </c>
+      <c r="K194" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="L194" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="M194" s="0" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="B195" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C195" s="0" t="n">
+        <v>34012</v>
+      </c>
+      <c r="D195" s="0" t="n">
+        <v>13800</v>
+      </c>
+      <c r="E195" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F195" s="0" t="n">
+        <v>76833</v>
+      </c>
+      <c r="I195" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J195" s="0" t="n">
+        <v>468</v>
+      </c>
+      <c r="K195" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="L195" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M195" s="0" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="B196" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C196" s="0" t="n">
+        <v>34012</v>
+      </c>
+      <c r="D196" s="0" t="n">
+        <v>13800</v>
+      </c>
+      <c r="E196" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F196" s="0" t="n">
+        <v>76833</v>
+      </c>
+      <c r="I196" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J196" s="0" t="n">
+        <v>468</v>
+      </c>
+      <c r="K196" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="L196" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M196" s="0" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="C197" s="3" t="n">
+        <v>34097</v>
+      </c>
+      <c r="D197" s="0" t="n">
+        <v>13800</v>
+      </c>
+      <c r="E197" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F197" s="3" t="n">
+        <v>76980</v>
+      </c>
+      <c r="I197" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J197" s="0" t="n">
+        <v>485</v>
+      </c>
+      <c r="K197" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="L197" s="0" t="n">
+        <v>4800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 22 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="407">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1232,6 +1232,15 @@
   </si>
   <si>
     <t xml:space="preserve">21.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240421184617/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240422153101/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1347,15 +1356,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M197"/>
+  <dimension ref="A1:M198"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2130" topLeftCell="A186" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="705" topLeftCell="A186" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M204" activeCellId="0" sqref="M204"/>
+      <selection pane="bottomLeft" activeCell="E202" activeCellId="0" sqref="E202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8617,6 +8626,44 @@
       </c>
       <c r="L197" s="0" t="n">
         <v>4800</v>
+      </c>
+      <c r="M197" s="0" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="B198" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="C198" s="0" t="n">
+        <v>34151</v>
+      </c>
+      <c r="D198" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E198" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F198" s="0" t="n">
+        <v>77084</v>
+      </c>
+      <c r="I198" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J198" s="0" t="n">
+        <v>486</v>
+      </c>
+      <c r="K198" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="L198" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M198" s="0" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 23 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="409">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1241,6 +1241,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240422153101/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240423144314/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1356,15 +1362,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M198"/>
+  <dimension ref="A1:M199"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="705" topLeftCell="A186" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1275" topLeftCell="A186" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E202" activeCellId="0" sqref="E202"/>
+      <selection pane="bottomLeft" activeCell="L199" activeCellId="0" sqref="L199"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8664,6 +8670,41 @@
       </c>
       <c r="M198" s="0" t="s">
         <v>406</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="C199" s="3" t="n">
+        <v>34183</v>
+      </c>
+      <c r="D199" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E199" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F199" s="3" t="n">
+        <v>77143</v>
+      </c>
+      <c r="I199" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J199" s="0" t="n">
+        <v>487</v>
+      </c>
+      <c r="K199" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="L199" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M199" s="0" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 24 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="411">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1247,6 +1247,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240423144314/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240424201459/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1362,15 +1368,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M199"/>
+  <dimension ref="A1:M200"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1275" topLeftCell="A186" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L199" activeCellId="0" sqref="L199"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="675" topLeftCell="A199" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="M200" activeCellId="0" sqref="M200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8705,6 +8711,41 @@
       </c>
       <c r="M199" s="0" t="s">
         <v>408</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="B200" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="C200" s="3" t="n">
+        <v>34262</v>
+      </c>
+      <c r="D200" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E200" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F200" s="0" t="n">
+        <v>77229</v>
+      </c>
+      <c r="I200" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J200" s="0" t="n">
+        <v>488</v>
+      </c>
+      <c r="K200" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="L200" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M200" s="0" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 25 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="413">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1253,6 +1253,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240424201459/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240425145543/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1368,15 +1374,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M200"/>
+  <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="675" topLeftCell="A199" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="M200" activeCellId="0" sqref="M200"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="765" topLeftCell="A199" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="M201" activeCellId="0" sqref="M201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8746,6 +8752,41 @@
       </c>
       <c r="M200" s="0" t="s">
         <v>410</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="C201" s="3" t="n">
+        <v>34262</v>
+      </c>
+      <c r="D201" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E201" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F201" s="0" t="n">
+        <v>77229</v>
+      </c>
+      <c r="I201" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J201" s="0" t="n">
+        <v>488</v>
+      </c>
+      <c r="K201" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="L201" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M201" s="0" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with data from 26 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="415">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1258,7 +1258,13 @@
     <t xml:space="preserve">25.04.2024</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20240425145543/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+    <t xml:space="preserve">https://web.archive.org/web/20240425230537/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240426204049/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1374,15 +1380,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M201"/>
+  <dimension ref="A1:M202"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="765" topLeftCell="A199" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M201" activeCellId="0" sqref="M201"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1380" topLeftCell="A199" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="K207" activeCellId="0" sqref="K207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8759,10 +8765,10 @@
         <v>411</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C201" s="3" t="n">
-        <v>34262</v>
+        <v>34305</v>
       </c>
       <c r="D201" s="0" t="n">
         <v>14500</v>
@@ -8771,22 +8777,57 @@
         <v>8400</v>
       </c>
       <c r="F201" s="0" t="n">
-        <v>77229</v>
+        <v>77293</v>
       </c>
       <c r="I201" s="0" t="n">
         <v>8000</v>
       </c>
       <c r="J201" s="0" t="n">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="K201" s="0" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L201" s="0" t="n">
         <v>4800</v>
       </c>
       <c r="M201" s="0" t="s">
         <v>412</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="C202" s="3" t="n">
+        <v>34356</v>
+      </c>
+      <c r="D202" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E202" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F202" s="3" t="n">
+        <v>77368</v>
+      </c>
+      <c r="I202" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J202" s="0" t="n">
+        <v>489</v>
+      </c>
+      <c r="K202" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L202" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M202" s="0" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data updated 28 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="419">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1265,6 +1265,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240426204049/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240427193549/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240428123712/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1380,15 +1392,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M202"/>
+  <dimension ref="A1:M204"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1380" topLeftCell="A199" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K207" activeCellId="0" sqref="K207"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="705" topLeftCell="A199" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="M204" activeCellId="0" sqref="M204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8828,6 +8840,76 @@
       </c>
       <c r="M202" s="0" t="s">
         <v>414</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="B203" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="C203" s="3" t="n">
+        <v>34356</v>
+      </c>
+      <c r="D203" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E203" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F203" s="3" t="n">
+        <v>77368</v>
+      </c>
+      <c r="I203" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J203" s="0" t="n">
+        <v>489</v>
+      </c>
+      <c r="K203" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L203" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M203" s="0" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="C204" s="3" t="n">
+        <v>34454</v>
+      </c>
+      <c r="D204" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E204" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F204" s="3" t="n">
+        <v>77575</v>
+      </c>
+      <c r="I204" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J204" s="0" t="n">
+        <v>491</v>
+      </c>
+      <c r="K204" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L204" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M204" s="0" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data updated 29 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="421">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1277,6 +1277,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240428123712/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240429163724/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1392,15 +1398,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M204"/>
+  <dimension ref="A1:M205"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="705" topLeftCell="A199" activePane="bottomLeft" state="split"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="735" topLeftCell="A199" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M204" activeCellId="0" sqref="M204"/>
+      <selection pane="bottomLeft" activeCell="I210" activeCellId="0" sqref="I210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8910,6 +8916,41 @@
       </c>
       <c r="M204" s="0" t="s">
         <v>418</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="C205" s="0" t="n">
+        <v>34488</v>
+      </c>
+      <c r="D205" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E205" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F205" s="0" t="n">
+        <v>77643</v>
+      </c>
+      <c r="I205" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J205" s="0" t="n">
+        <v>491</v>
+      </c>
+      <c r="K205" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L205" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M205" s="0" t="s">
+        <v>420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data updated 30 April 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="423">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1283,6 +1283,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240429163724/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.04.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240430124840/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1398,15 +1404,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M205"/>
+  <dimension ref="A1:M206"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="735" topLeftCell="A199" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1320" topLeftCell="A199" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I210" activeCellId="0" sqref="I210"/>
+      <selection pane="bottomLeft" activeCell="L206" activeCellId="0" sqref="L206"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8951,6 +8957,41 @@
       </c>
       <c r="M205" s="0" t="s">
         <v>420</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="C206" s="3" t="n">
+        <v>34535</v>
+      </c>
+      <c r="D206" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E206" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F206" s="3" t="n">
+        <v>77704</v>
+      </c>
+      <c r="I206" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J206" s="0" t="n">
+        <v>492</v>
+      </c>
+      <c r="K206" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L206" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M206" s="0" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data updated 1 May 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="425">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1289,6 +1289,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240430124840/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240501161201/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1404,15 +1410,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M206"/>
+  <dimension ref="A1:M207"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1320" topLeftCell="A199" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="795" topLeftCell="A199" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L206" activeCellId="0" sqref="L206"/>
+      <selection pane="bottomLeft" activeCell="M207" activeCellId="0" sqref="M207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8992,6 +8998,41 @@
       </c>
       <c r="M206" s="0" t="s">
         <v>422</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="C207" s="3" t="n">
+        <v>34568</v>
+      </c>
+      <c r="D207" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E207" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F207" s="0" t="n">
+        <v>77765</v>
+      </c>
+      <c r="I207" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J207" s="0" t="n">
+        <v>492</v>
+      </c>
+      <c r="K207" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L207" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M207" s="0" t="s">
+        <v>424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data updated 06 May 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="434">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1295,6 +1295,33 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240501161201/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240502164235/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240503142834/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240504232915/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240505201358/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240506141604/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1410,15 +1437,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M207"/>
+  <dimension ref="A1:M212"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="795" topLeftCell="A199" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="870" topLeftCell="A199" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M207" activeCellId="0" sqref="M207"/>
+      <selection pane="bottomLeft" activeCell="M211" activeCellId="0" sqref="M211"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -9033,6 +9060,181 @@
       </c>
       <c r="M207" s="0" t="s">
         <v>424</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="C208" s="3" t="n">
+        <v>34596</v>
+      </c>
+      <c r="D208" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E208" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F208" s="0" t="n">
+        <v>77816</v>
+      </c>
+      <c r="I208" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J208" s="0" t="n">
+        <v>492</v>
+      </c>
+      <c r="K208" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L208" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M208" s="0" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="B209" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="C209" s="0" t="n">
+        <v>34622</v>
+      </c>
+      <c r="D209" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E209" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F209" s="0" t="n">
+        <v>77867</v>
+      </c>
+      <c r="I209" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J209" s="0" t="n">
+        <v>492</v>
+      </c>
+      <c r="K209" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L209" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M209" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="C210" s="0" t="n">
+        <v>34622</v>
+      </c>
+      <c r="D210" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E210" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F210" s="0" t="n">
+        <v>77867</v>
+      </c>
+      <c r="I210" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J210" s="0" t="n">
+        <v>492</v>
+      </c>
+      <c r="K210" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L210" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M210" s="0" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B211" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="C211" s="0" t="n">
+        <v>34622</v>
+      </c>
+      <c r="D211" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E211" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F211" s="0" t="n">
+        <v>77867</v>
+      </c>
+      <c r="I211" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J211" s="0" t="n">
+        <v>492</v>
+      </c>
+      <c r="K211" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L211" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M211" s="0" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="C212" s="0" t="n">
+        <v>34735</v>
+      </c>
+      <c r="D212" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="E212" s="0" t="n">
+        <v>8400</v>
+      </c>
+      <c r="F212" s="0" t="n">
+        <v>78108</v>
+      </c>
+      <c r="I212" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J212" s="0" t="n">
+        <v>497</v>
+      </c>
+      <c r="K212" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L212" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="M212" s="0" t="s">
+        <v>433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated up to 12 May 2024
</commit_message>
<xml_diff>
--- a/data/mortality_data.xlsx
+++ b/data/mortality_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="446">
   <si>
     <t xml:space="preserve">tracker_date</t>
   </si>
@@ -1322,6 +1322,42 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20240506141604/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240507213334/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240508193156/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240509235238/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240510225527/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240511211611/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.05.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20240512182431/https://www.aljazeera.com/news/longform/2023/10/9/israel-hamas-war-in-maps-and-charts-live-tracker</t>
   </si>
 </sst>
 </file>
@@ -1437,15 +1473,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M212"/>
+  <dimension ref="A1:M218"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="870" topLeftCell="A199" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M211" activeCellId="0" sqref="M211"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="960" topLeftCell="A209" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="M218" activeCellId="0" sqref="M218"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -9235,6 +9271,198 @@
       </c>
       <c r="M212" s="0" t="s">
         <v>433</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="C213" s="3" t="n">
+        <v>34789</v>
+      </c>
+      <c r="D213" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="F213" s="0" t="n">
+        <v>78204</v>
+      </c>
+      <c r="I213" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J213" s="0" t="n">
+        <v>498</v>
+      </c>
+      <c r="K213" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L213" s="0" t="n">
+        <v>4950</v>
+      </c>
+      <c r="M213" s="0" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="C214" s="3" t="n">
+        <v>34789</v>
+      </c>
+      <c r="D214" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="F214" s="0" t="n">
+        <v>78204</v>
+      </c>
+      <c r="I214" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J214" s="0" t="n">
+        <v>498</v>
+      </c>
+      <c r="K214" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L214" s="0" t="n">
+        <v>4950</v>
+      </c>
+      <c r="M214" s="0" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="B215" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="C215" s="0" t="n">
+        <v>34904</v>
+      </c>
+      <c r="D215" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="F215" s="0" t="n">
+        <v>78514</v>
+      </c>
+      <c r="I215" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J215" s="0" t="n">
+        <v>498</v>
+      </c>
+      <c r="K215" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L215" s="0" t="n">
+        <v>4950</v>
+      </c>
+      <c r="M215" s="0" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="B216" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C216" s="0" t="n">
+        <v>34904</v>
+      </c>
+      <c r="D216" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="F216" s="0" t="n">
+        <v>78514</v>
+      </c>
+      <c r="I216" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J216" s="0" t="n">
+        <v>498</v>
+      </c>
+      <c r="K216" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L216" s="0" t="n">
+        <v>4950</v>
+      </c>
+      <c r="M216" s="0" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="B217" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C217" s="0" t="n">
+        <v>34904</v>
+      </c>
+      <c r="D217" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="F217" s="0" t="n">
+        <v>78514</v>
+      </c>
+      <c r="I217" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J217" s="0" t="n">
+        <v>498</v>
+      </c>
+      <c r="K217" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L217" s="0" t="n">
+        <v>4950</v>
+      </c>
+      <c r="M217" s="0" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="C218" s="3" t="n">
+        <v>35034</v>
+      </c>
+      <c r="D218" s="0" t="n">
+        <v>14500</v>
+      </c>
+      <c r="F218" s="0" t="n">
+        <v>78755</v>
+      </c>
+      <c r="I218" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="J218" s="0" t="n">
+        <v>498</v>
+      </c>
+      <c r="K218" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="L218" s="0" t="n">
+        <v>4950</v>
+      </c>
+      <c r="M218" s="0" t="s">
+        <v>445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>